<commit_message>
Diem danh ngay 23/2
</commit_message>
<xml_diff>
--- a/trunk/Điểm danh.xlsx
+++ b/trunk/Điểm danh.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="9">
   <si>
     <t xml:space="preserve">                  Ngày
 Tên</t>
@@ -580,7 +580,7 @@
   <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,6 +677,9 @@
       <c r="F4" s="13" t="s">
         <v>8</v>
       </c>
+      <c r="G4" s="13" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:19" s="13" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
@@ -704,6 +707,9 @@
       <c r="E6" s="13" t="s">
         <v>8</v>
       </c>
+      <c r="G6" s="13" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:19" s="16" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
@@ -717,6 +723,9 @@
         <v>8</v>
       </c>
       <c r="E7" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="16" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
diem danh ngay 24
</commit_message>
<xml_diff>
--- a/trunk/Điểm danh.xlsx
+++ b/trunk/Điểm danh.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="9">
   <si>
     <t xml:space="preserve">                  Ngày
 Tên</t>
@@ -580,15 +580,15 @@
   <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" style="9" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="8" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="4" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -613,7 +613,9 @@
       <c r="G1" s="3">
         <v>40991</v>
       </c>
-      <c r="H1" s="3"/>
+      <c r="H1" s="3">
+        <v>40992</v>
+      </c>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -648,6 +650,9 @@
       <c r="G2" s="13" t="s">
         <v>8</v>
       </c>
+      <c r="H2" s="13" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:19" s="13" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -668,6 +673,9 @@
       <c r="G3" s="13" t="s">
         <v>8</v>
       </c>
+      <c r="H3" s="13" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:19" s="13" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -680,6 +688,9 @@
       <c r="G4" s="13" t="s">
         <v>8</v>
       </c>
+      <c r="H4" s="13" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:19" s="13" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
@@ -692,6 +703,9 @@
       <c r="G5" s="13" t="s">
         <v>8</v>
       </c>
+      <c r="H5" s="13" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:19" s="13" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
@@ -710,6 +724,9 @@
       <c r="G6" s="13" t="s">
         <v>8</v>
       </c>
+      <c r="H6" s="13" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:19" s="16" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
@@ -726,6 +743,9 @@
         <v>8</v>
       </c>
       <c r="G7" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="16" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>